<commit_message>
Add Government Document Number columns to example input files
</commit_message>
<xml_diff>
--- a/inputs/search_worldcat/example.xlsx
+++ b/inputs/search_worldcat/example.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25019"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E53BE6E4-0929-4A6B-B9BE-A9C9F2711D2A}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC45BE17-DCF0-4C2C-AAA0-9F3FAAFB5EAD}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>mms_id</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>issn</t>
+  </si>
+  <si>
+    <t>gpo_item_num_074</t>
+  </si>
+  <si>
+    <t>gov_doc_class_num_086</t>
   </si>
 </sst>
 </file>
@@ -82,10 +88,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:N1048576"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -411,9 +418,11 @@
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,6 +437,12 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>